<commit_message>
Excel generator to database on script
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -1,76 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\Vista\vista\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C490659-A742-4377-86CD-825EF43BCD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9778CC9-A12D-452A-B320-440C69174853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">10. 4. </t>
-  </si>
-  <si>
-    <t>datum OD kdy je menu</t>
-  </si>
-  <si>
-    <t>datum DO kdy je menu</t>
-  </si>
-  <si>
-    <t>24. 4.</t>
-  </si>
-  <si>
-    <t>menu číslo 1</t>
-  </si>
-  <si>
-    <t>menu číslo 2</t>
-  </si>
-  <si>
-    <t>menu číslo 3</t>
-  </si>
-  <si>
-    <t>menu číslo 4</t>
-  </si>
-  <si>
-    <t>menu číslo 5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Segedinský guláš podávaný s houskovým knedlíkem / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
   </si>
   <si>
-    <t>pondělní polévka</t>
-  </si>
-  <si>
     <t>Krůtí steak po staročesku s jasmínovou rýží / Old-czech style turkey breast with jasmine rice</t>
   </si>
   <si>
@@ -83,18 +42,6 @@
     <t>Pečený candát se zeleninou na másle podávaný s pteržel. Brambory / Baked zander with vegetables in butter served with parsley potatoes</t>
   </si>
   <si>
-    <t>úterní polévka</t>
-  </si>
-  <si>
-    <t>středeční polévka</t>
-  </si>
-  <si>
-    <t>čtvrteční polévka</t>
-  </si>
-  <si>
-    <t>páteční polévka</t>
-  </si>
-  <si>
     <t>Bramborová polévka / Potato soup</t>
   </si>
   <si>
@@ -108,6 +55,42 @@
   </si>
   <si>
     <t>Státní svátek. Denní menu nepodáváme. / Bank holiday. We do not serve daily menu.</t>
+  </si>
+  <si>
+    <t>Od</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>1, 3, 7</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>1, 3 ,7</t>
+  </si>
+  <si>
+    <t>4, 7</t>
+  </si>
+  <si>
+    <t>1, 3, 7, 9</t>
+  </si>
+  <si>
+    <t>Alergen_Jidlo</t>
+  </si>
+  <si>
+    <t>Alergen_Polivka</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>Polivka</t>
+  </si>
+  <si>
+    <t>Jidlo</t>
   </si>
 </sst>
 </file>
@@ -139,7 +122,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +141,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -167,34 +174,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,116 +532,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEB1CD8-C190-4190-B49D-32A6CCBAB5D7}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CB9550-EC31-43C2-B332-E514BA3C8745}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="166.85546875" customWidth="1"/>
+    <col min="1" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>45761</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45765</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="D3">
+        <v>95</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D4">
+        <v>95</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>150</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated popup and parsing excel with day of the week
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\Vista\vista\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9778CC9-A12D-452A-B320-440C69174853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A231ABE-AEB9-4056-A4C1-27C4D4BCF1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Segedinský guláš podávaný s houskovým knedlíkem / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Jidlo</t>
+  </si>
+  <si>
+    <t>Cislo_dne</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CB9550-EC31-43C2-B332-E514BA3C8745}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,9 +549,10 @@
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -570,13 +574,16 @@
       <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45761</v>
+        <v>45767</v>
       </c>
       <c r="B2" s="9">
-        <v>45765</v>
+        <v>45772</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
@@ -593,8 +600,11 @@
       <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="7" t="s">
@@ -609,8 +619,11 @@
       <c r="G3" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="7" t="s">
@@ -628,8 +641,11 @@
       <c r="G4" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
@@ -647,8 +663,11 @@
       <c r="G5" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
@@ -662,6 +681,9 @@
       </c>
       <c r="F6" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: refactor Order to database
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\Vista\vista\vista\vista-app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A231ABE-AEB9-4056-A4C1-27C4D4BCF1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7671F6E6-E888-45E3-8F5E-15C7C738F4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,10 +580,10 @@
     </row>
     <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45767</v>
+        <v>45810</v>
       </c>
       <c r="B2" s="9">
-        <v>45772</v>
+        <v>45814</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
add: Menu and loading gif before the menu is fully loaded
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7671F6E6-E888-45E3-8F5E-15C7C738F4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE93C943-129E-483F-B141-357E2D497C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -27,36 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>Segedinský guláš podávaný s houskovým knedlíkem / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
-  </si>
-  <si>
-    <t>Krůtí steak po staročesku s jasmínovou rýží / Old-czech style turkey breast with jasmine rice</t>
-  </si>
-  <si>
-    <t>Grilovaná pljeskavica s opékanými brambory a pikantním ajvarem / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
-  </si>
-  <si>
-    <t>Tagliolini s hovězí svíčkovou sypané sýrem Grana Padano / Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
-  </si>
-  <si>
-    <t>Pečený candát se zeleninou na másle podávaný s pteržel. Brambory / Baked zander with vegetables in butter served with parsley potatoes</t>
-  </si>
-  <si>
-    <t>Bramborová polévka / Potato soup</t>
-  </si>
-  <si>
-    <t>Čočková polévka s párkem / Lentil soup with sausages</t>
-  </si>
-  <si>
-    <t>Hovězí vývar s masem a nudlemi / Beef consommé with meat and noodles</t>
-  </si>
-  <si>
-    <t>Minestrone polévka s těstovinami / Minestrone soup with pasta</t>
-  </si>
-  <si>
-    <t>Státní svátek. Denní menu nepodáváme. / Bank holiday. We do not serve daily menu.</t>
-  </si>
-  <si>
     <t>Od</t>
   </si>
   <si>
@@ -94,6 +64,36 @@
   </si>
   <si>
     <t>Cislo_dne</t>
+  </si>
+  <si>
+    <t>Vepřová panenka s pepřovou omáčkou a knedlíkem / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
+  </si>
+  <si>
+    <t>Krůtí prsa s bramborem/ Old-czech style turkey breast with jasmine rice</t>
+  </si>
+  <si>
+    <t>Koprová omáčka se sázeným vejcem / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
+  </si>
+  <si>
+    <t>Pasta La Vista / Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
+  </si>
+  <si>
+    <t>Losos na kmíně  / Baked zander with vegetables in butter served with parsley potatoes</t>
+  </si>
+  <si>
+    <t>Rajčatová polévka / Potato soup</t>
+  </si>
+  <si>
+    <t>Kuřecí vývar / Lentil soup with sausages</t>
+  </si>
+  <si>
+    <t>Pórková polévka / Beef consommé with meat and noodles</t>
+  </si>
+  <si>
+    <t>Těstovinová polévka / Minestrone soup with pasta</t>
+  </si>
+  <si>
+    <t>Hovězí vývarovka / Bank holiday. We do not serve daily menu.</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,51 +554,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45810</v>
+        <v>45817</v>
       </c>
       <c r="B2" s="9">
-        <v>45814</v>
+        <v>45821</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>80</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -608,16 +608,16 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="7" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>95</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -627,19 +627,19 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>95</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -649,19 +649,19 @@
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -671,16 +671,16 @@
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>150</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H6">
         <v>5</v>

</xml_diff>

<commit_message>
add: SignIn form with surname
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE93C943-129E-483F-B141-357E2D497C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A4374F-5AF6-4F54-9B01-C98B6190A2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -66,34 +66,34 @@
     <t>Cislo_dne</t>
   </si>
   <si>
-    <t>Vepřová panenka s pepřovou omáčkou a knedlíkem / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
-  </si>
-  <si>
-    <t>Krůtí prsa s bramborem/ Old-czech style turkey breast with jasmine rice</t>
-  </si>
-  <si>
-    <t>Koprová omáčka se sázeným vejcem / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
-  </si>
-  <si>
-    <t>Pasta La Vista / Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
-  </si>
-  <si>
-    <t>Losos na kmíně  / Baked zander with vegetables in butter served with parsley potatoes</t>
-  </si>
-  <si>
-    <t>Rajčatová polévka / Potato soup</t>
-  </si>
-  <si>
-    <t>Kuřecí vývar / Lentil soup with sausages</t>
-  </si>
-  <si>
-    <t>Pórková polévka / Beef consommé with meat and noodles</t>
-  </si>
-  <si>
-    <t>Těstovinová polévka / Minestrone soup with pasta</t>
-  </si>
-  <si>
-    <t>Hovězí vývarovka / Bank holiday. We do not serve daily menu.</t>
+    <t>Jídlo 1 Nevim co už dál / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
+  </si>
+  <si>
+    <t>Jídlo 2 Nevim co už dál / Old-czech style turkey breast with jasmine rice</t>
+  </si>
+  <si>
+    <t>Jídlo 3 Jídlo Nevim co už dál / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
+  </si>
+  <si>
+    <t>Jídlo 4 Nevim co už dál/ Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
+  </si>
+  <si>
+    <t>Jídlo 5 Nevim co už dál  / Baked zander with vegetables in butter served with parsley potatoes</t>
+  </si>
+  <si>
+    <t>Mlsná polévka / Potato soup</t>
+  </si>
+  <si>
+    <t>Kuřecí vývarov / Lentil soup with sausages</t>
+  </si>
+  <si>
+    <t>Porek / Beef consommé with meat and noodles</t>
+  </si>
+  <si>
+    <t>Best polívka / Minestrone soup with pasta</t>
+  </si>
+  <si>
+    <t>Pátková polívka / Bank holiday. We do not serve daily menu.</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,10 +580,10 @@
     </row>
     <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45817</v>
+        <v>45859</v>
       </c>
       <c r="B2" s="9">
-        <v>45821</v>
+        <v>45863</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add: Excel Export with tommorows orders
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A4374F-5AF6-4F54-9B01-C98B6190A2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666C939-F41A-47C6-8EFF-8C56E37203BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -66,34 +66,34 @@
     <t>Cislo_dne</t>
   </si>
   <si>
-    <t>Jídlo 1 Nevim co už dál / Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
-  </si>
-  <si>
-    <t>Jídlo 2 Nevim co už dál / Old-czech style turkey breast with jasmine rice</t>
-  </si>
-  <si>
-    <t>Jídlo 3 Jídlo Nevim co už dál / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
-  </si>
-  <si>
-    <t>Jídlo 4 Nevim co už dál/ Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
-  </si>
-  <si>
-    <t>Jídlo 5 Nevim co už dál  / Baked zander with vegetables in butter served with parsley potatoes</t>
-  </si>
-  <si>
-    <t>Mlsná polévka / Potato soup</t>
-  </si>
-  <si>
-    <t>Kuřecí vývarov / Lentil soup with sausages</t>
-  </si>
-  <si>
-    <t>Porek / Beef consommé with meat and noodles</t>
-  </si>
-  <si>
-    <t>Best polívka / Minestrone soup with pasta</t>
-  </si>
-  <si>
-    <t>Pátková polívka / Bank holiday. We do not serve daily menu.</t>
+    <t>Food 111/ Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
+  </si>
+  <si>
+    <t>Food 222 / Old-czech style turkey breast with jasmine rice</t>
+  </si>
+  <si>
+    <t>Foood 333 / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
+  </si>
+  <si>
+    <t>Food 444 / Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
+  </si>
+  <si>
+    <t>Foood 555  / Baked zander with vegetables in butter served with parsley potatoes</t>
+  </si>
+  <si>
+    <t>5555 polívka / Bank holiday. We do not serve daily menu.</t>
+  </si>
+  <si>
+    <t>4444 polívka / Minestrone soup with pasta</t>
+  </si>
+  <si>
+    <t>33333 / Beef consommé with meat and noodles</t>
+  </si>
+  <si>
+    <t>2222/ Lentil soup with sausages</t>
+  </si>
+  <si>
+    <t>Mlsná 111 polévka 111 / Potato soup</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,10 +580,10 @@
     </row>
     <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45859</v>
+        <v>45866</v>
       </c>
       <c r="B2" s="9">
-        <v>45863</v>
+        <v>45870</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>6</v>
@@ -614,7 +614,7 @@
         <v>95</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>6</v>
@@ -658,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>6</v>
@@ -680,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H6">
         <v>5</v>

</xml_diff>

<commit_message>
add: Security on admin pages
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666C939-F41A-47C6-8EFF-8C56E37203BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8A9BEB-B66A-437A-AF71-C2F5F304B264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,10 +580,10 @@
     </row>
     <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45866</v>
+        <v>45901</v>
       </c>
       <c r="B2" s="9">
-        <v>45870</v>
+        <v>45905</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add: Admin adding special dates, updated logic on displaying meals and menu
</commit_message>
<xml_diff>
--- a/vista-app/public/menu.xlsx
+++ b/vista-app/public/menu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danus\Desktop\VistaAppka\vista\vista-app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\React\vista-frontend\vista\vista-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9131875-84A9-4514-AE51-B31DE7ECD9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046ECF0-EF08-44A5-8CAC-CE4AEF8AE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{992A0FB4-8BD1-410B-879E-BF5A835259EC}"/>
   </bookViews>
   <sheets>
     <sheet name="List2" sheetId="2" r:id="rId1"/>
@@ -66,34 +66,34 @@
     <t>Cislo_dne</t>
   </si>
   <si>
-    <t>Food 111/ Traditional Hungarian goulash with pork meat and sauerkraut served with bread dumplings</t>
-  </si>
-  <si>
-    <t>Food 222 / Old-czech style turkey breast with jasmine rice</t>
-  </si>
-  <si>
-    <t>Foood 333 / Grilled minced meat with roasted potatoes and spicy salad of roasted peppers</t>
-  </si>
-  <si>
-    <t>Food 444 / Tagliolini with beef tenderloin sprinkled with Grana Padano Cheese</t>
-  </si>
-  <si>
-    <t>Foood 555  / Baked zander with vegetables in butter served with parsley potatoes</t>
-  </si>
-  <si>
-    <t>5555 polívka / Bank holiday. We do not serve daily menu.</t>
-  </si>
-  <si>
-    <t>4444 polívka / Minestrone soup with pasta</t>
-  </si>
-  <si>
-    <t>33333 / Beef consommé with meat and noodles</t>
-  </si>
-  <si>
-    <t>2222/ Lentil soup with sausages</t>
-  </si>
-  <si>
-    <t>Mlsná 111 polévka 111 / Potato soup</t>
+    <t>Něměcký Řízek s bramborovou kaší / English name</t>
+  </si>
+  <si>
+    <t>Český řízek s bramborovou kaší / English name</t>
+  </si>
+  <si>
+    <t>Maďarský guláš / English name</t>
+  </si>
+  <si>
+    <t>Pečený candát na másle / English name</t>
+  </si>
+  <si>
+    <t>Srbská pljeskavica / English name</t>
+  </si>
+  <si>
+    <t>Německá polévka</t>
+  </si>
+  <si>
+    <t>Česká polévka</t>
+  </si>
+  <si>
+    <t>Maďarská polévka</t>
+  </si>
+  <si>
+    <t>Švédská polévka</t>
+  </si>
+  <si>
+    <t>Srbská polévka</t>
   </si>
 </sst>
 </file>
@@ -193,13 +193,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,20 +539,20 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="1" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,113 +578,113 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="94.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>45901</v>
-      </c>
-      <c r="B2" s="7">
-        <v>45905</v>
-      </c>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>45908</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45912</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>80</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8">
+        <v>95</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8">
+        <v>95</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8">
+        <v>150</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="8">
+        <v>150</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="9">
-        <v>95</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="9">
-        <v>95</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9">
-        <v>150</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="9">
-        <v>150</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8">
         <v>5</v>
       </c>
     </row>

</xml_diff>